<commit_message>
Switched Quit and Exit commands and documentation. Quit closes the Adventurer; Exit leaves a Building and returns to the Town view.
</commit_message>
<xml_diff>
--- a/ChronosLib/PM/RTM.xlsx
+++ b/ChronosLib/PM/RTM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20800" windowHeight="17200" tabRatio="500"/>
+    <workbookView xWindow="10060" yWindow="40" windowWidth="17120" windowHeight="17400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TA00" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -487,9 +487,6 @@
     <t>Test Passed</t>
   </si>
   <si>
-    <t>UC00b. Exit Adventurer</t>
-  </si>
-  <si>
     <t>Paths</t>
   </si>
   <si>
@@ -511,10 +508,19 @@
     <t xml:space="preserve">Terminate the Adventurer program. </t>
   </si>
   <si>
-    <t>N01. Save Hero at current location, close registries, and terminate program from Exit menu option or Window close (red) button.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E01. Exit command does not terminate program.  </t>
+    <t>UC00b. Quit Adventurer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N01. Quit program with Adventure not open. </t>
+  </si>
+  <si>
+    <t>N02. From menu: Quit program with Adventure open. Save Hero at current location, close registries, and terminate program.</t>
+  </si>
+  <si>
+    <t>N03. From Window close event: Quit program. Save Hero at current location, close registries, and terminate program.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N04. Restart program from last save point, with Hero in proper Building. </t>
   </si>
 </sst>
 </file>
@@ -634,7 +640,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -682,6 +688,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
@@ -726,56 +746,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -809,6 +829,13 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -823,6 +850,13 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1152,22 +1186,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13" style="20" customWidth="1"/>
-    <col min="2" max="3" width="30.33203125" style="19" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="20"/>
-    <col min="6" max="16384" width="10.83203125" style="21"/>
+    <col min="1" max="1" width="13" style="17" customWidth="1"/>
+    <col min="2" max="3" width="30.33203125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="17"/>
+    <col min="6" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18"/>
+      <c r="A1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="26">
       <c r="A2" s="7" t="s">
@@ -1177,7 +1211,7 @@
         <v>132</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>134</v>
@@ -1187,74 +1221,92 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="78">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="21">
+        <v>41874</v>
+      </c>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="39">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C4" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="21">
+        <v>41854</v>
+      </c>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" ht="39">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="24">
+        <v>41854</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" s="27" customFormat="1" ht="16" customHeight="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:5" ht="26">
+      <c r="A7" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="24">
-        <v>41874</v>
-      </c>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" ht="39">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="24">
-        <v>41854</v>
-      </c>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:5" ht="39">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="27">
-        <v>41854</v>
-      </c>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" s="30" customFormat="1" ht="16" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:5" ht="52">
-      <c r="A7" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:5" ht="26">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="52">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" ht="52">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" ht="39">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1325,36 +1377,36 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="72">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="29" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="30">
         <v>41339</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="48">
-      <c r="A6" s="16"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" ht="84">
       <c r="A7" s="11" t="s">
@@ -1483,30 +1535,30 @@
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="72">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="29" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="24">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" ht="36">
       <c r="A17" s="11" t="s">
@@ -1524,43 +1576,43 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="48">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="30">
         <v>41339</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="29"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="15"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="1:7" ht="24">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:7" ht="96">
       <c r="A21" s="11" t="s">
@@ -2068,11 +2120,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
@@ -2085,6 +2132,11 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated RTM and minor doc additions.
</commit_message>
<xml_diff>
--- a/ChronosLib/PM/RTM.xlsx
+++ b/ChronosLib/PM/RTM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="40" windowWidth="17120" windowHeight="17400" tabRatio="500"/>
+    <workbookView xWindow="7140" yWindow="3940" windowWidth="15900" windowHeight="9560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TA00" sheetId="1" r:id="rId1"/>
@@ -496,9 +496,6 @@
     <t>The player can also display the About box or general Help from the menu.</t>
   </si>
   <si>
-    <t>N03. Display About dialog with accredidations</t>
-  </si>
-  <si>
     <t>N02. Display Help window from menu or F1 key</t>
   </si>
   <si>
@@ -521,13 +518,16 @@
   </si>
   <si>
     <t xml:space="preserve">N04. Restart program from last save point, with Hero in proper Building. </t>
+  </si>
+  <si>
+    <t>N03. Display About dialog with accreditations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -590,11 +590,6 @@
       <sz val="11"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -640,7 +635,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -703,8 +698,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -767,9 +766,6 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -786,16 +782,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -836,6 +832,8 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -857,6 +855,8 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1228,7 +1228,7 @@
         <v>137</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" s="21">
         <v>41874</v>
@@ -1241,12 +1241,14 @@
         <v>138</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="21">
         <v>41854</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="21">
+        <v>41854</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="39">
       <c r="A5" s="19"/>
@@ -1254,47 +1256,57 @@
         <v>138</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="24">
+        <v>147</v>
+      </c>
+      <c r="D5" s="23">
         <v>41854</v>
       </c>
-      <c r="E5" s="19"/>
-    </row>
-    <row r="6" spans="1:5" s="27" customFormat="1" ht="16" customHeight="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="E5" s="23">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="26" customFormat="1" ht="16" customHeight="1">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" ht="26">
       <c r="A7" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="21">
+        <v>41875</v>
+      </c>
+      <c r="E7" s="21">
+        <v>41875</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="52">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+        <v>144</v>
+      </c>
+      <c r="D8" s="23">
+        <v>41875</v>
+      </c>
+      <c r="E8" s="23">
+        <v>41875</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="52">
       <c r="A9" s="19"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -1303,7 +1315,7 @@
       <c r="A10" s="19"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1380,33 +1392,33 @@
       <c r="A5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>41339</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="48">
       <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7" ht="84">
       <c r="A7" s="11" t="s">
@@ -1538,27 +1550,27 @@
       <c r="A15" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="24">
       <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" ht="36">
       <c r="A17" s="11" t="s">
@@ -1579,40 +1591,40 @@
       <c r="A18" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <v>41339</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="29"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="29"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="24">
       <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="96">
       <c r="A21" s="11" t="s">
@@ -2120,6 +2132,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
@@ -2132,11 +2149,6 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated EXIT, ENTER and RETURN use cases, with updates to UX00_PortalOpeningView and UX03_AdventureTownView.
</commit_message>
<xml_diff>
--- a/ChronosLib/PM/RTM.xlsx
+++ b/ChronosLib/PM/RTM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>N03. Display About dialog with accreditations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -782,10 +785,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1188,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1308,7 +1311,9 @@
       <c r="C9" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="23" t="s">
+        <v>148</v>
+      </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" ht="39">
@@ -1389,11 +1394,11 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="72">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="B5" s="28"/>
+      <c r="C5" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -1405,12 +1410,12 @@
       <c r="F5" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" ht="48">
-      <c r="A6" s="28"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1423,7 @@
       <c r="F6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" ht="84">
       <c r="A7" s="11" t="s">
@@ -1547,30 +1552,30 @@
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="72">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" ht="24">
-      <c r="A16" s="28"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" ht="36">
       <c r="A17" s="11" t="s">
@@ -1588,14 +1593,14 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="48">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="29">
@@ -1604,27 +1609,27 @@
       <c r="F18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="28"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="29"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="27"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" ht="24">
-      <c r="A20" s="28"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="29"/>
       <c r="F20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" ht="96">
       <c r="A21" s="11" t="s">
@@ -2132,11 +2137,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
@@ -2149,6 +2149,11 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Removed the RTM test tab.
</commit_message>
<xml_diff>
--- a/ChronosLib/PM/RTM.xlsx
+++ b/ChronosLib/PM/RTM.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UC00a_Initialize" sheetId="1" r:id="rId1"/>
     <sheet name="UC00b_Quit" sheetId="4" r:id="rId2"/>
-    <sheet name="testTab" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Use Case</t>
   </si>
@@ -817,117 +816,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="13" style="3" customWidth="1"/>
-    <col min="2" max="3" width="30.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18" style="3" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="3"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="20">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" ht="26">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="312">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7">
-        <v>41875</v>
-      </c>
-      <c r="F3" s="7">
-        <v>41875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="52">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9">
-        <v>41875</v>
-      </c>
-      <c r="F4" s="9">
-        <v>41875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="52">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="39">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>

</xml_diff>